<commit_message>
amenity list, mongodb documents
</commit_message>
<xml_diff>
--- a/doc/poi.xlsx
+++ b/doc/poi.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="96">
   <si>
     <t>Type</t>
   </si>
@@ -41,7 +41,7 @@
     <t>bar</t>
   </si>
   <si>
-    <t> name=*</t>
+    <t>name=*</t>
   </si>
   <si>
     <t>Bar is a purpose-built commercial establishment that sells alcoholic drinks to be consumed on the premises. They are characterised by a noisy and vibrant atmosphere, similar to a party and usually don't sell food. See also the description of the tags amenity=pub;bar;restaurant for a distinction between these.</t>
@@ -50,7 +50,7 @@
     <t>bbq</t>
   </si>
   <si>
-    <t>     covered=yes/no -- default is no.
+    <t>covered=yes/no -- default is no.
     fuel=wood/electric/charcoal</t>
   </si>
   <si>
@@ -107,19 +107,16 @@
     amenity=fast_food
     name=Westgate Fisheries
     cuisine=fish_and_chips
-For other types of cuisines check cuisine= please. </t>
-  </si>
-  <si>
-    <t>Fast food restaurant (see also amenity=restaurant). The kind of food served can be tagged with cuisine=* and diet=*. </t>
+For other types of cuisines check cuisine= please.</t>
+  </si>
+  <si>
+    <t>Fast food restaurant (see also amenity=restaurant). The kind of food served can be tagged with cuisine=* and diet=*.</t>
   </si>
   <si>
     <t>food_court</t>
   </si>
   <si>
-    <t>name=*</t>
-  </si>
-  <si>
-    <t>An area with several different restaurant food counters and a shared eating area. Commonly found in malls, airports, etc. </t>
+    <t>An area with several different restaurant food counters and a shared eating area. Commonly found in malls, airports, etc.</t>
   </si>
   <si>
     <t>ice_cream</t>
@@ -168,7 +165,7 @@
     cuisine=fish_and_chips</t>
   </si>
   <si>
-    <t>Restaurant (not fast food, see amenity=fast_food). The kind of food served can be tagged with cuisine=* and diet=*. </t>
+    <t>Restaurant (not fast food, see amenity=fast_food). The kind of food served can be tagged with cuisine=* and diet=*.</t>
   </si>
   <si>
     <t>Education</t>
@@ -198,6 +195,20 @@
     <t>bicycle_parking</t>
   </si>
   <si>
+    <t>Tag 	Description
+name=* 	Larger areas of bike parking may be named.
+operator=* 	Cycle parking may be operated by some organisation.
+covered=* 	Parked bikes are protected from rain.
+access=* 	Public access is implied in most roadside cases. Some bike racks can be private to a university, company, or other organisation, possibly requiring keys or codes to access.
+capacity=* 	The number of bikes that can be parked here.
+fee=* 	In some places, one must pay to park one's bike.
+    paid is a less widespread alias for this.
+bicycle_parking=* 	Details the type of bicycle parking (e.g. stands, wall loops...).
+cyclestreets_id=* 	A link to the ID (e.g. 12345) of the location describing a photo of the cycle parking in CycleStreets. Multiple IDs should be separated by semi-colons.
+maxstay=* 	Maximum time the bicycle is allowed to be parked at that place - given sometimes at covered parking-places.
+surveillance=* 	Closed-circuit television (CCTV) security cameras can be marked with this. See the linked page for details of the values in use. Depending on the layout, a separate node nearby may be enough.</t>
+  </si>
+  <si>
     <t>bicycle_repair_station</t>
   </si>
   <si>
@@ -210,7 +221,7 @@
     <t>bus_station</t>
   </si>
   <si>
-    <t>Has been replaced by public_transport=station. </t>
+    <t>Has been replaced by public_transport=station.</t>
   </si>
   <si>
     <t>http://wiki.openstreetmap.org/wiki/Key:public_transport</t>
@@ -228,7 +239,7 @@
     <t>ev_charging</t>
   </si>
   <si>
-    <t>Electric vehicle charging facility. Don't use, amenity=charging_station is preferred. </t>
+    <t>Electric vehicle charging facility. Don't use, amenity=charging_station is preferred.</t>
   </si>
   <si>
     <t>charging_station</t>
@@ -243,7 +254,7 @@
     <t>grit_bin</t>
   </si>
   <si>
-    <t>A container that holds grit or a mixture of salt and grit. </t>
+    <t>A container that holds grit or a mixture of salt and grit.</t>
   </si>
   <si>
     <t>motorcycle_parking</t>
@@ -252,7 +263,7 @@
     <t>parking</t>
   </si>
   <si>
-    <t>Car park. Nodes and areas (without access tag) will get a parking symbol. Areas will be coloured. Streets on car parking are often tagged highway=service and service=parking_aisle. </t>
+    <t>Car park. Nodes and areas (without access tag) will get a parking symbol. Areas will be coloured. Streets on car parking are often tagged highway=service and service=parking_aisle.</t>
   </si>
   <si>
     <t>http://wiki.openstreetmap.org/wiki/Tag:highway%3Dservice
@@ -262,13 +273,13 @@
     <t>parking_entrance</t>
   </si>
   <si>
-    <t>An entrance or exit to an underground or multi-storey parking facility. Group multiple parking entrances together with a relation using the tags type=site and site=parking. Do not mix with amenity=parking. </t>
+    <t>An entrance or exit to an underground or multi-storey parking facility. Group multiple parking entrances together with a relation using the tags type=site and site=parking. Do not mix with amenity=parking.</t>
   </si>
   <si>
     <t>parking_space</t>
   </si>
   <si>
-    <t>A single parking space. Group multiple parking spaces together with a relation using the tags type=site and site=parking. Do not mix with amenity=parking. </t>
+    <t>A single parking space. Group multiple parking spaces together with a relation using the tags type=site and site=parking. Do not mix with amenity=parking.</t>
   </si>
   <si>
     <t>taxi</t>
@@ -303,7 +314,7 @@
     <t>arts_centre</t>
   </si>
   <si>
-    <t>    name=*
+    <t>name=*
     description=*
     Operator=*</t>
   </si>
@@ -317,7 +328,7 @@
     <t>cinema</t>
   </si>
   <si>
-    <t>     name=* - The name of the cinema
+    <t>name=* - The name of the cinema
     operator=* - The organisation / brand operating the cinema
     building=cinema - To describe the type of building
     drive_in=yes/no - To indicate if a cinema is a drive-in cinema. See Wikipedia:Drive-in theater for more information.
@@ -336,7 +347,7 @@
     <t>fountain</t>
   </si>
   <si>
-    <t>     name=* - The name of the fountain.
+    <t>name=* - The name of the fountain.
     drinking_water=yes/no - Indication whether a feature provides drinking water
     lit=yes/no - Are there lights shining on/in the fountain?</t>
   </si>
@@ -421,7 +432,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -449,11 +460,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -526,15 +532,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -610,9 +616,9 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
+      <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -691,6 +697,7 @@
       <c r="B6" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="D6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
@@ -708,97 +715,117 @@
         <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>30</v>
-      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>32</v>
-      </c>
+      <c r="D13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>33</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>34</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>35</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="B20" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="D20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
         <v>40</v>
       </c>
+      <c r="D21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>41</v>
       </c>
+      <c r="D22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="D23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
@@ -815,16 +842,19 @@
       <c r="B25" s="0" t="s">
         <v>46</v>
       </c>
+      <c r="D25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
         <v>47</v>
       </c>
+      <c r="D26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
         <v>48</v>
       </c>
+      <c r="D27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
@@ -838,16 +868,19 @@
       <c r="B29" s="0" t="s">
         <v>51</v>
       </c>
+      <c r="D29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="D30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
         <v>53</v>
       </c>
+      <c r="D31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
@@ -861,6 +894,7 @@
       <c r="B33" s="0" t="s">
         <v>56</v>
       </c>
+      <c r="D33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
@@ -931,7 +965,7 @@
         <v>73</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,7 +1007,7 @@
         <v>82</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -994,7 +1028,7 @@
         <v>86</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1010,7 +1044,7 @@
         <v>89</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="359.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
UT osm file parsing
</commit_message>
<xml_diff>
--- a/doc/poi.xlsx
+++ b/doc/poi.xlsx
@@ -5,20 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="205" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="205" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Aerialway" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Aeroway" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Amenity" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Data" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="UT-amenity1" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="108">
   <si>
     <t>Type</t>
   </si>
@@ -423,6 +424,42 @@
   </si>
   <si>
     <t>lat="50.0567548" lon="19.9081330"</t>
+  </si>
+  <si>
+    <t>amenity</t>
+  </si>
+  <si>
+    <t>highway</t>
+  </si>
+  <si>
+    <t>turism</t>
+  </si>
+  <si>
+    <t>hist</t>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>historic</t>
+  </si>
+  <si>
+    <t>memorial</t>
+  </si>
+  <si>
+    <t>tourism</t>
+  </si>
+  <si>
+    <t>hostel</t>
+  </si>
+  <si>
+    <t>pharmacy</t>
+  </si>
+  <si>
+    <t>museum</t>
+  </si>
+  <si>
+    <t>all count</t>
   </si>
 </sst>
 </file>
@@ -469,20 +506,51 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0099FF"/>
+        <bgColor rgb="FF0066CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF420E"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3DEB3D"/>
+        <bgColor rgb="FF33CCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -511,7 +579,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -544,6 +612,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -553,6 +637,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF3DEB3D"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0099FF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -615,7 +759,7 @@
   </sheetPr>
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
@@ -697,6 +841,7 @@
       <c r="B6" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="C6" s="0"/>
       <c r="D6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -753,6 +898,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0"/>
       <c r="D12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -762,39 +908,46 @@
       <c r="B13" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="C13" s="0"/>
       <c r="D13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
         <v>32</v>
       </c>
+      <c r="C14" s="0"/>
       <c r="D14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
         <v>33</v>
       </c>
+      <c r="C15" s="0"/>
       <c r="D15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="C16" s="0"/>
       <c r="D16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
         <v>35</v>
       </c>
+      <c r="C17" s="0"/>
       <c r="D17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="C18" s="0"/>
       <c r="D18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0"/>
       <c r="D19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -813,24 +966,28 @@
       <c r="B21" s="0" t="s">
         <v>40</v>
       </c>
+      <c r="C21" s="0"/>
       <c r="D21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>41</v>
       </c>
+      <c r="C22" s="0"/>
       <c r="D22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="C23" s="0"/>
       <c r="D23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
         <v>43</v>
       </c>
+      <c r="C24" s="0"/>
       <c r="D24" s="1" t="s">
         <v>44</v>
       </c>
@@ -842,24 +999,28 @@
       <c r="B25" s="0" t="s">
         <v>46</v>
       </c>
+      <c r="C25" s="0"/>
       <c r="D25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
         <v>47</v>
       </c>
+      <c r="C26" s="0"/>
       <c r="D26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
         <v>48</v>
       </c>
+      <c r="C27" s="0"/>
       <c r="D27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="C28" s="0"/>
       <c r="D28" s="1" t="s">
         <v>50</v>
       </c>
@@ -868,24 +1029,28 @@
       <c r="B29" s="0" t="s">
         <v>51</v>
       </c>
+      <c r="C29" s="0"/>
       <c r="D29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="C30" s="0"/>
       <c r="D30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
         <v>53</v>
       </c>
+      <c r="C31" s="0"/>
       <c r="D31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
         <v>54</v>
       </c>
+      <c r="C32" s="0"/>
       <c r="D32" s="1" t="s">
         <v>55</v>
       </c>
@@ -894,12 +1059,14 @@
       <c r="B33" s="0" t="s">
         <v>56</v>
       </c>
+      <c r="C33" s="0"/>
       <c r="D33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="C34" s="0"/>
       <c r="D34" s="1" t="s">
         <v>58</v>
       </c>
@@ -911,6 +1078,7 @@
       <c r="B35" s="0" t="s">
         <v>60</v>
       </c>
+      <c r="C35" s="0"/>
       <c r="D35" s="1" t="s">
         <v>61</v>
       </c>
@@ -919,6 +1087,7 @@
       <c r="B36" s="0" t="s">
         <v>62</v>
       </c>
+      <c r="C36" s="0"/>
       <c r="D36" s="1" t="s">
         <v>63</v>
       </c>
@@ -927,6 +1096,10 @@
       <c r="B37" s="0" t="s">
         <v>64</v>
       </c>
+      <c r="C37" s="0"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
@@ -943,11 +1116,16 @@
       <c r="B40" s="0" t="s">
         <v>68</v>
       </c>
+      <c r="C40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
         <v>69</v>
       </c>
+      <c r="C41" s="0"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
@@ -972,6 +1150,7 @@
       <c r="B45" s="0" t="s">
         <v>74</v>
       </c>
+      <c r="C45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
@@ -1001,6 +1180,7 @@
       <c r="B49" s="0" t="s">
         <v>81</v>
       </c>
+      <c r="C49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
@@ -1014,6 +1194,7 @@
       <c r="B51" s="0" t="s">
         <v>83</v>
       </c>
+      <c r="C51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
@@ -1172,4 +1353,290 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8"/>
+      <c r="C1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0" t="n">
+        <f aca="false">SUM(C2:C22)</f>
+        <v>11</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <f aca="false">SUM(D2:D21)</f>
+        <v>2</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <f aca="false">SUM(E2:E21)</f>
+        <v>2</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <f aca="false">SUM(F2:F21)</f>
+        <v>1</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <f aca="false">SUM(G2:G21)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <f aca="false">SUM(C23:G23)-G23</f>
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>